<commit_message>
Menambahkan kolom baru di halaman kendaraan
</commit_message>
<xml_diff>
--- a/media/laporan/2025/07/data-kendaraan-20250703-20250703.xlsx
+++ b/media/laporan/2025/07/data-kendaraan-20250703-20250703.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>DATA KENDARAAN</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Availability</t>
+  </si>
+  <si>
+    <t>Tanggal</t>
   </si>
   <si>
     <t>Status</t>
@@ -472,10 +475,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A11" sqref="A11:J11"/>
+      <selection activeCell="A11" sqref="A11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -492,7 +495,7 @@
     <col min="10" max="10" width="25" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -506,7 +509,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -520,7 +523,7 @@
       <c r="I2"/>
       <c r="J2"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -551,10 +554,13 @@
       <c r="J10" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="K10" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -564,13 +570,14 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="7"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A11:K11"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>